<commit_message>
- Fixed: LD logging - Added: post-migration packages - Added: check-connection package
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/Location-DataPatch-2024-12-01.xlsx
+++ b/Integration Services Project2/notes/Location-DataPatch-2024-12-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBF5BA0-F5E6-4E84-89A8-7004BA5498F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99AC115-4C1E-4094-9816-5951748DDBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{B478EE47-66DE-4FC6-997B-86B6C737A3E6}"/>
   </bookViews>
@@ -2769,7 +2769,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2791,6 +2791,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2859,7 +2865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2950,29 +2956,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3454,7 +3453,7 @@
       <c r="A1" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>595</v>
       </c>
     </row>
@@ -3462,7 +3461,7 @@
       <c r="A2" s="23" t="s">
         <v>594</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="39"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
@@ -5043,7 +5042,7 @@
       <c r="I1" t="s">
         <v>869</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="34" t="s">
         <v>99</v>
       </c>
       <c r="K1" t="s">
@@ -5085,7 +5084,7 @@
         <f>A2</f>
         <v>PGC</v>
       </c>
-      <c r="J2" s="39" t="str">
+      <c r="J2" s="35" t="str">
         <f>C2</f>
         <v>01</v>
       </c>
@@ -5126,7 +5125,7 @@
         <f t="shared" ref="I3:I66" si="2">A3</f>
         <v>PGC</v>
       </c>
-      <c r="J3" s="39" t="str">
+      <c r="J3" s="35" t="str">
         <f t="shared" ref="J3:J66" si="3">C3</f>
         <v>B1</v>
       </c>
@@ -5167,7 +5166,7 @@
         <f t="shared" si="2"/>
         <v>PGC</v>
       </c>
-      <c r="J4" s="39" t="str">
+      <c r="J4" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -5208,7 +5207,7 @@
         <f t="shared" si="2"/>
         <v>PGC</v>
       </c>
-      <c r="J5" s="39" t="str">
+      <c r="J5" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -5249,7 +5248,7 @@
         <f t="shared" si="2"/>
         <v>PGC</v>
       </c>
-      <c r="J6" s="39" t="str">
+      <c r="J6" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B4</v>
       </c>
@@ -5290,7 +5289,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J7" s="39" t="str">
+      <c r="J7" s="35" t="str">
         <f t="shared" si="3"/>
         <v>04</v>
       </c>
@@ -5331,7 +5330,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J8" s="39" t="str">
+      <c r="J8" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -5372,7 +5371,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J9" s="39" t="str">
+      <c r="J9" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -5413,7 +5412,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J10" s="39" t="str">
+      <c r="J10" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -5454,7 +5453,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J11" s="39" t="str">
+      <c r="J11" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -5495,7 +5494,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J12" s="39" t="str">
+      <c r="J12" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -5536,7 +5535,7 @@
         <f t="shared" si="2"/>
         <v>SKG</v>
       </c>
-      <c r="J13" s="39" t="str">
+      <c r="J13" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -5577,7 +5576,7 @@
         <f t="shared" si="2"/>
         <v>SKG</v>
       </c>
-      <c r="J14" s="39" t="str">
+      <c r="J14" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -5618,7 +5617,7 @@
         <f t="shared" si="2"/>
         <v>SKG</v>
       </c>
-      <c r="J15" s="39" t="str">
+      <c r="J15" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -5659,7 +5658,7 @@
         <f t="shared" si="2"/>
         <v>SKG</v>
       </c>
-      <c r="J16" s="39" t="str">
+      <c r="J16" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -5700,7 +5699,7 @@
         <f t="shared" si="2"/>
         <v>BGK</v>
       </c>
-      <c r="J17" s="39" t="str">
+      <c r="J17" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -5741,7 +5740,7 @@
         <f t="shared" si="2"/>
         <v>BGK</v>
       </c>
-      <c r="J18" s="39" t="str">
+      <c r="J18" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -5782,7 +5781,7 @@
         <f t="shared" si="2"/>
         <v>BGK</v>
       </c>
-      <c r="J19" s="39" t="str">
+      <c r="J19" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -5823,7 +5822,7 @@
         <f t="shared" si="2"/>
         <v>BGK</v>
       </c>
-      <c r="J20" s="39" t="str">
+      <c r="J20" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -5864,7 +5863,7 @@
         <f t="shared" si="2"/>
         <v>HGN</v>
       </c>
-      <c r="J21" s="39" t="str">
+      <c r="J21" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -5905,7 +5904,7 @@
         <f t="shared" si="2"/>
         <v>HGN</v>
       </c>
-      <c r="J22" s="39" t="str">
+      <c r="J22" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -5946,7 +5945,7 @@
         <f t="shared" si="2"/>
         <v>HGN</v>
       </c>
-      <c r="J23" s="39" t="str">
+      <c r="J23" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -5987,7 +5986,7 @@
         <f t="shared" si="2"/>
         <v>HGN</v>
       </c>
-      <c r="J24" s="39" t="str">
+      <c r="J24" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -6028,7 +6027,7 @@
         <f t="shared" si="2"/>
         <v>KVN</v>
       </c>
-      <c r="J25" s="39" t="str">
+      <c r="J25" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -6069,7 +6068,7 @@
         <f t="shared" si="2"/>
         <v>KVN</v>
       </c>
-      <c r="J26" s="39" t="str">
+      <c r="J26" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -6110,7 +6109,7 @@
         <f t="shared" si="2"/>
         <v>KVN</v>
       </c>
-      <c r="J27" s="39" t="str">
+      <c r="J27" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -6151,7 +6150,7 @@
         <f t="shared" si="2"/>
         <v>KVN</v>
       </c>
-      <c r="J28" s="39" t="str">
+      <c r="J28" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -6192,7 +6191,7 @@
         <f t="shared" si="2"/>
         <v>SER</v>
       </c>
-      <c r="J29" s="39" t="str">
+      <c r="J29" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -6233,7 +6232,7 @@
         <f t="shared" si="2"/>
         <v>SER</v>
       </c>
-      <c r="J30" s="39" t="str">
+      <c r="J30" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -6274,7 +6273,7 @@
         <f t="shared" si="2"/>
         <v>SER</v>
       </c>
-      <c r="J31" s="39" t="str">
+      <c r="J31" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -6315,7 +6314,7 @@
         <f t="shared" si="2"/>
         <v>SER</v>
       </c>
-      <c r="J32" s="39" t="str">
+      <c r="J32" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -6356,7 +6355,7 @@
         <f t="shared" si="2"/>
         <v>WLH</v>
       </c>
-      <c r="J33" s="39" t="str">
+      <c r="J33" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -6397,7 +6396,7 @@
         <f t="shared" si="2"/>
         <v>WLH</v>
       </c>
-      <c r="J34" s="39" t="str">
+      <c r="J34" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -6438,7 +6437,7 @@
         <f t="shared" si="2"/>
         <v>WLH</v>
       </c>
-      <c r="J35" s="39" t="str">
+      <c r="J35" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -6479,7 +6478,7 @@
         <f t="shared" si="2"/>
         <v>WLH</v>
       </c>
-      <c r="J36" s="39" t="str">
+      <c r="J36" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -6520,7 +6519,7 @@
         <f t="shared" si="2"/>
         <v>PTP</v>
       </c>
-      <c r="J37" s="39" t="str">
+      <c r="J37" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -6561,7 +6560,7 @@
         <f t="shared" si="2"/>
         <v>PTP</v>
       </c>
-      <c r="J38" s="39" t="str">
+      <c r="J38" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -6602,7 +6601,7 @@
         <f t="shared" si="2"/>
         <v>PTP</v>
       </c>
-      <c r="J39" s="39" t="str">
+      <c r="J39" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -6643,7 +6642,7 @@
         <f t="shared" si="2"/>
         <v>PTP</v>
       </c>
-      <c r="J40" s="39" t="str">
+      <c r="J40" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -6684,7 +6683,7 @@
         <f t="shared" si="2"/>
         <v>BNK</v>
       </c>
-      <c r="J41" s="39" t="str">
+      <c r="J41" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -6725,7 +6724,7 @@
         <f t="shared" si="2"/>
         <v>BNK</v>
       </c>
-      <c r="J42" s="39" t="str">
+      <c r="J42" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -6766,7 +6765,7 @@
         <f t="shared" si="2"/>
         <v>BNK</v>
       </c>
-      <c r="J43" s="39" t="str">
+      <c r="J43" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -6807,7 +6806,7 @@
         <f t="shared" si="2"/>
         <v>BNK</v>
       </c>
-      <c r="J44" s="39" t="str">
+      <c r="J44" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -6848,7 +6847,7 @@
         <f t="shared" si="2"/>
         <v>FRP</v>
       </c>
-      <c r="J45" s="39" t="str">
+      <c r="J45" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -6889,7 +6888,7 @@
         <f t="shared" si="2"/>
         <v>FRP</v>
       </c>
-      <c r="J46" s="39" t="str">
+      <c r="J46" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -6930,7 +6929,7 @@
         <f t="shared" si="2"/>
         <v>FRP</v>
       </c>
-      <c r="J47" s="39" t="str">
+      <c r="J47" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -6971,7 +6970,7 @@
         <f t="shared" si="2"/>
         <v>FRP</v>
       </c>
-      <c r="J48" s="39" t="str">
+      <c r="J48" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -7012,7 +7011,7 @@
         <f t="shared" si="2"/>
         <v>LTI</v>
       </c>
-      <c r="J49" s="39" t="str">
+      <c r="J49" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -7053,7 +7052,7 @@
         <f t="shared" si="2"/>
         <v>LTI</v>
       </c>
-      <c r="J50" s="39" t="str">
+      <c r="J50" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -7094,7 +7093,7 @@
         <f t="shared" si="2"/>
         <v>LTI</v>
       </c>
-      <c r="J51" s="39" t="str">
+      <c r="J51" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -7135,7 +7134,7 @@
         <f t="shared" si="2"/>
         <v>LTI</v>
       </c>
-      <c r="J52" s="39" t="str">
+      <c r="J52" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -7176,7 +7175,7 @@
         <f t="shared" si="2"/>
         <v>DBG</v>
       </c>
-      <c r="J53" s="39" t="str">
+      <c r="J53" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -7217,7 +7216,7 @@
         <f t="shared" si="2"/>
         <v>DBG</v>
       </c>
-      <c r="J54" s="39" t="str">
+      <c r="J54" s="35" t="str">
         <f t="shared" si="3"/>
         <v>M</v>
       </c>
@@ -7258,7 +7257,7 @@
         <f t="shared" si="2"/>
         <v>DBG</v>
       </c>
-      <c r="J55" s="39" t="str">
+      <c r="J55" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -7299,7 +7298,7 @@
         <f t="shared" si="2"/>
         <v>DBG</v>
       </c>
-      <c r="J56" s="39" t="str">
+      <c r="J56" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -7340,7 +7339,7 @@
         <f t="shared" si="2"/>
         <v>DBG</v>
       </c>
-      <c r="J57" s="39" t="str">
+      <c r="J57" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -7381,7 +7380,7 @@
         <f t="shared" si="2"/>
         <v>DBG</v>
       </c>
-      <c r="J58" s="39" t="str">
+      <c r="J58" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B4</v>
       </c>
@@ -7422,7 +7421,7 @@
         <f t="shared" si="2"/>
         <v>DBG</v>
       </c>
-      <c r="J59" s="39" t="str">
+      <c r="J59" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B5</v>
       </c>
@@ -7463,7 +7462,7 @@
         <f t="shared" si="2"/>
         <v>DBG</v>
       </c>
-      <c r="J60" s="39" t="str">
+      <c r="J60" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B6</v>
       </c>
@@ -7504,7 +7503,7 @@
         <f t="shared" si="2"/>
         <v>CQY</v>
       </c>
-      <c r="J61" s="39" t="str">
+      <c r="J61" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -7545,7 +7544,7 @@
         <f t="shared" si="2"/>
         <v>CQY</v>
       </c>
-      <c r="J62" s="39" t="str">
+      <c r="J62" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B1</v>
       </c>
@@ -7586,7 +7585,7 @@
         <f t="shared" si="2"/>
         <v>CQY</v>
       </c>
-      <c r="J63" s="39" t="str">
+      <c r="J63" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B2</v>
       </c>
@@ -7627,7 +7626,7 @@
         <f t="shared" si="2"/>
         <v>CQY</v>
       </c>
-      <c r="J64" s="39" t="str">
+      <c r="J64" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B3</v>
       </c>
@@ -7668,7 +7667,7 @@
         <f t="shared" si="2"/>
         <v>CQY</v>
       </c>
-      <c r="J65" s="39" t="str">
+      <c r="J65" s="35" t="str">
         <f t="shared" si="3"/>
         <v>B4</v>
       </c>
@@ -7709,7 +7708,7 @@
         <f t="shared" si="2"/>
         <v>CNT</v>
       </c>
-      <c r="J66" s="39" t="str">
+      <c r="J66" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -7743,15 +7742,15 @@
         <v>111</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" ref="H67:H99" si="6">CONCATENATE(B67," Station - Level ",C67)</f>
+        <f t="shared" ref="H67:H82" si="6">CONCATENATE(B67," Station - Level ",C67)</f>
         <v>Chinatown Station - Level B1</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I99" si="7">A67</f>
         <v>CNT</v>
       </c>
-      <c r="J67" s="39" t="str">
-        <f t="shared" ref="J67:J99" si="8">C67</f>
+      <c r="J67" s="35" t="str">
+        <f t="shared" ref="J67:J82" si="8">C67</f>
         <v>B1</v>
       </c>
       <c r="L67" t="str">
@@ -7791,7 +7790,7 @@
         <f t="shared" si="7"/>
         <v>CNT</v>
       </c>
-      <c r="J68" s="39" t="str">
+      <c r="J68" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B2</v>
       </c>
@@ -7832,7 +7831,7 @@
         <f t="shared" si="7"/>
         <v>CNT</v>
       </c>
-      <c r="J69" s="39" t="str">
+      <c r="J69" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B3</v>
       </c>
@@ -7873,7 +7872,7 @@
         <f t="shared" si="7"/>
         <v>OTP</v>
       </c>
-      <c r="J70" s="39" t="str">
+      <c r="J70" s="35" t="str">
         <f t="shared" si="8"/>
         <v>01</v>
       </c>
@@ -7914,7 +7913,7 @@
         <f t="shared" si="7"/>
         <v>OTP</v>
       </c>
-      <c r="J71" s="39" t="str">
+      <c r="J71" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B1</v>
       </c>
@@ -7955,7 +7954,7 @@
         <f t="shared" si="7"/>
         <v>OTP</v>
       </c>
-      <c r="J72" s="39" t="str">
+      <c r="J72" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B2</v>
       </c>
@@ -7996,7 +7995,7 @@
         <f t="shared" si="7"/>
         <v>OTP</v>
       </c>
-      <c r="J73" s="39" t="str">
+      <c r="J73" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B3</v>
       </c>
@@ -8037,7 +8036,7 @@
         <f t="shared" si="7"/>
         <v>OTP</v>
       </c>
-      <c r="J74" s="39" t="str">
+      <c r="J74" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B4</v>
       </c>
@@ -8078,7 +8077,7 @@
         <f t="shared" si="7"/>
         <v>OTP</v>
       </c>
-      <c r="J75" s="39" t="str">
+      <c r="J75" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B5</v>
       </c>
@@ -8119,7 +8118,7 @@
         <f t="shared" si="7"/>
         <v>HBF</v>
       </c>
-      <c r="J76" s="39" t="str">
+      <c r="J76" s="35" t="str">
         <f t="shared" si="8"/>
         <v>01</v>
       </c>
@@ -8160,7 +8159,7 @@
         <f t="shared" si="7"/>
         <v>HBF</v>
       </c>
-      <c r="J77" s="39" t="str">
+      <c r="J77" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B1</v>
       </c>
@@ -8201,7 +8200,7 @@
         <f t="shared" si="7"/>
         <v>HBF</v>
       </c>
-      <c r="J78" s="39" t="str">
+      <c r="J78" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B2</v>
       </c>
@@ -8242,7 +8241,7 @@
         <f t="shared" si="7"/>
         <v>HBF</v>
       </c>
-      <c r="J79" s="39" t="str">
+      <c r="J79" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B3</v>
       </c>
@@ -8283,7 +8282,7 @@
         <f t="shared" si="7"/>
         <v>XPFB</v>
       </c>
-      <c r="J80" s="39" t="str">
+      <c r="J80" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B1</v>
       </c>
@@ -8324,7 +8323,7 @@
         <f t="shared" si="7"/>
         <v>XPFB</v>
       </c>
-      <c r="J81" s="39" t="str">
+      <c r="J81" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B2</v>
       </c>
@@ -8365,7 +8364,7 @@
         <f t="shared" si="7"/>
         <v>XPFB</v>
       </c>
-      <c r="J82" s="39" t="str">
+      <c r="J82" s="35" t="str">
         <f t="shared" si="8"/>
         <v>B3</v>
       </c>
@@ -8403,7 +8402,7 @@
         <f t="shared" si="7"/>
         <v>PGC</v>
       </c>
-      <c r="J83" s="39"/>
+      <c r="J83" s="35"/>
       <c r="L83" t="str">
         <f t="shared" si="9"/>
         <v>PGC</v>
@@ -8438,7 +8437,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J84" s="39"/>
+      <c r="J84" s="35"/>
       <c r="L84" t="str">
         <f t="shared" si="9"/>
         <v>PGL</v>
@@ -8473,7 +8472,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J85" s="39"/>
+      <c r="J85" s="35"/>
       <c r="L85" t="str">
         <f t="shared" si="9"/>
         <v>SKG</v>
@@ -8508,7 +8507,7 @@
         <f t="shared" si="7"/>
         <v>BGK</v>
       </c>
-      <c r="J86" s="39"/>
+      <c r="J86" s="35"/>
       <c r="L86" t="str">
         <f t="shared" si="9"/>
         <v>BGK</v>
@@ -8543,7 +8542,7 @@
         <f t="shared" si="7"/>
         <v>HGN</v>
       </c>
-      <c r="J87" s="39"/>
+      <c r="J87" s="35"/>
       <c r="L87" t="str">
         <f t="shared" si="9"/>
         <v>HGN</v>
@@ -8578,7 +8577,7 @@
         <f t="shared" si="7"/>
         <v>KVN</v>
       </c>
-      <c r="J88" s="39"/>
+      <c r="J88" s="35"/>
       <c r="L88" t="str">
         <f t="shared" si="9"/>
         <v>KVN</v>
@@ -8613,7 +8612,7 @@
         <f t="shared" si="7"/>
         <v>SER</v>
       </c>
-      <c r="J89" s="39"/>
+      <c r="J89" s="35"/>
       <c r="L89" t="str">
         <f t="shared" si="9"/>
         <v>SER</v>
@@ -8648,7 +8647,7 @@
         <f t="shared" si="7"/>
         <v>WLH</v>
       </c>
-      <c r="J90" s="39"/>
+      <c r="J90" s="35"/>
       <c r="L90" t="str">
         <f t="shared" si="9"/>
         <v>WLH</v>
@@ -8683,7 +8682,7 @@
         <f t="shared" si="7"/>
         <v>PTP</v>
       </c>
-      <c r="J91" s="39"/>
+      <c r="J91" s="35"/>
       <c r="L91" t="str">
         <f t="shared" si="9"/>
         <v>PTP</v>
@@ -8718,7 +8717,7 @@
         <f t="shared" si="7"/>
         <v>BNK</v>
       </c>
-      <c r="J92" s="39"/>
+      <c r="J92" s="35"/>
       <c r="L92" t="str">
         <f t="shared" si="9"/>
         <v>BNK</v>
@@ -8753,7 +8752,7 @@
         <f t="shared" si="7"/>
         <v>FRP</v>
       </c>
-      <c r="J93" s="39"/>
+      <c r="J93" s="35"/>
       <c r="L93" t="str">
         <f t="shared" si="9"/>
         <v>FRP</v>
@@ -8788,7 +8787,7 @@
         <f t="shared" si="7"/>
         <v>LTI</v>
       </c>
-      <c r="J94" s="39"/>
+      <c r="J94" s="35"/>
       <c r="L94" t="str">
         <f t="shared" si="9"/>
         <v>LTI</v>
@@ -8823,7 +8822,7 @@
         <f t="shared" si="7"/>
         <v>DBG</v>
       </c>
-      <c r="J95" s="39"/>
+      <c r="J95" s="35"/>
       <c r="L95" t="str">
         <f t="shared" si="9"/>
         <v>DBG</v>
@@ -8858,7 +8857,7 @@
         <f t="shared" si="7"/>
         <v>CQY</v>
       </c>
-      <c r="J96" s="39"/>
+      <c r="J96" s="35"/>
       <c r="L96" t="str">
         <f t="shared" si="9"/>
         <v>CQY</v>
@@ -8893,7 +8892,7 @@
         <f t="shared" si="7"/>
         <v>CNT</v>
       </c>
-      <c r="J97" s="39"/>
+      <c r="J97" s="35"/>
       <c r="L97" t="str">
         <f t="shared" si="9"/>
         <v>CNT</v>
@@ -8928,7 +8927,7 @@
         <f t="shared" si="7"/>
         <v>OTP</v>
       </c>
-      <c r="J98" s="39"/>
+      <c r="J98" s="35"/>
       <c r="L98" t="str">
         <f t="shared" si="9"/>
         <v>OTP</v>
@@ -8963,7 +8962,7 @@
         <f t="shared" si="7"/>
         <v>HBF</v>
       </c>
-      <c r="J99" s="39"/>
+      <c r="J99" s="35"/>
       <c r="L99" t="str">
         <f t="shared" si="9"/>
         <v>HBF</v>
@@ -25133,8 +25132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6904B14-4EF6-478F-93F3-B83C8601A6EE}">
   <dimension ref="A1:M2734"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25175,7 +25174,7 @@
       <c r="I1" t="s">
         <v>869</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="34" t="s">
         <v>99</v>
       </c>
       <c r="K1" t="s">
@@ -25216,7 +25215,7 @@
         <f>A2</f>
         <v>SE1</v>
       </c>
-      <c r="J2" s="39" t="str">
+      <c r="J2" s="35" t="str">
         <f>C2</f>
         <v>01</v>
       </c>
@@ -25253,7 +25252,7 @@
         <f t="shared" ref="I3:I66" si="2">A3</f>
         <v>SE1</v>
       </c>
-      <c r="J3" s="39" t="str">
+      <c r="J3" s="35" t="str">
         <f t="shared" ref="J3:J66" si="3">C3</f>
         <v>02</v>
       </c>
@@ -25290,7 +25289,7 @@
         <f t="shared" si="2"/>
         <v>SE1</v>
       </c>
-      <c r="J4" s="39" t="str">
+      <c r="J4" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -25327,7 +25326,7 @@
         <f t="shared" si="2"/>
         <v>SE2</v>
       </c>
-      <c r="J5" s="39" t="str">
+      <c r="J5" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -25364,7 +25363,7 @@
         <f t="shared" si="2"/>
         <v>SE2</v>
       </c>
-      <c r="J6" s="39" t="str">
+      <c r="J6" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -25401,7 +25400,7 @@
         <f t="shared" si="2"/>
         <v>SE2</v>
       </c>
-      <c r="J7" s="39" t="str">
+      <c r="J7" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -25438,7 +25437,7 @@
         <f t="shared" si="2"/>
         <v>SE3</v>
       </c>
-      <c r="J8" s="39" t="str">
+      <c r="J8" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -25475,7 +25474,7 @@
         <f t="shared" si="2"/>
         <v>SE3</v>
       </c>
-      <c r="J9" s="39" t="str">
+      <c r="J9" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -25512,7 +25511,7 @@
         <f t="shared" si="2"/>
         <v>SE3</v>
       </c>
-      <c r="J10" s="39" t="str">
+      <c r="J10" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -25549,7 +25548,7 @@
         <f t="shared" si="2"/>
         <v>SE4</v>
       </c>
-      <c r="J11" s="39" t="str">
+      <c r="J11" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -25586,7 +25585,7 @@
         <f t="shared" si="2"/>
         <v>SE4</v>
       </c>
-      <c r="J12" s="39" t="str">
+      <c r="J12" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -25623,7 +25622,7 @@
         <f t="shared" si="2"/>
         <v>SE4</v>
       </c>
-      <c r="J13" s="39" t="str">
+      <c r="J13" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -25660,7 +25659,7 @@
         <f t="shared" si="2"/>
         <v>SE5</v>
       </c>
-      <c r="J14" s="39" t="str">
+      <c r="J14" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -25697,7 +25696,7 @@
         <f t="shared" si="2"/>
         <v>SE5</v>
       </c>
-      <c r="J15" s="39" t="str">
+      <c r="J15" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -25734,7 +25733,7 @@
         <f t="shared" si="2"/>
         <v>SE5</v>
       </c>
-      <c r="J16" s="39" t="str">
+      <c r="J16" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -25771,7 +25770,7 @@
         <f t="shared" si="2"/>
         <v>SW1</v>
       </c>
-      <c r="J17" s="39" t="str">
+      <c r="J17" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -25808,7 +25807,7 @@
         <f t="shared" si="2"/>
         <v>SW1</v>
       </c>
-      <c r="J18" s="39" t="str">
+      <c r="J18" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -25845,7 +25844,7 @@
         <f t="shared" si="2"/>
         <v>SW1</v>
       </c>
-      <c r="J19" s="39" t="str">
+      <c r="J19" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -25882,7 +25881,7 @@
         <f t="shared" si="2"/>
         <v>SW2</v>
       </c>
-      <c r="J20" s="39" t="str">
+      <c r="J20" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -25919,7 +25918,7 @@
         <f t="shared" si="2"/>
         <v>SW2</v>
       </c>
-      <c r="J21" s="39" t="str">
+      <c r="J21" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -25956,7 +25955,7 @@
         <f t="shared" si="2"/>
         <v>SW2</v>
       </c>
-      <c r="J22" s="39" t="str">
+      <c r="J22" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -25993,7 +25992,7 @@
         <f t="shared" si="2"/>
         <v>SW3</v>
       </c>
-      <c r="J23" s="39" t="str">
+      <c r="J23" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26030,7 +26029,7 @@
         <f t="shared" si="2"/>
         <v>SW3</v>
       </c>
-      <c r="J24" s="39" t="str">
+      <c r="J24" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26067,7 +26066,7 @@
         <f t="shared" si="2"/>
         <v>SW3</v>
       </c>
-      <c r="J25" s="39" t="str">
+      <c r="J25" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -26104,7 +26103,7 @@
         <f t="shared" si="2"/>
         <v>SW4</v>
       </c>
-      <c r="J26" s="39" t="str">
+      <c r="J26" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26141,7 +26140,7 @@
         <f t="shared" si="2"/>
         <v>SW4</v>
       </c>
-      <c r="J27" s="39" t="str">
+      <c r="J27" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26178,7 +26177,7 @@
         <f t="shared" si="2"/>
         <v>SW4</v>
       </c>
-      <c r="J28" s="39" t="str">
+      <c r="J28" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -26215,7 +26214,7 @@
         <f t="shared" si="2"/>
         <v>SW5</v>
       </c>
-      <c r="J29" s="39" t="str">
+      <c r="J29" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26252,7 +26251,7 @@
         <f t="shared" si="2"/>
         <v>SW5</v>
       </c>
-      <c r="J30" s="39" t="str">
+      <c r="J30" s="35" t="str">
         <f t="shared" si="3"/>
         <v>M</v>
       </c>
@@ -26289,7 +26288,7 @@
         <f t="shared" si="2"/>
         <v>SW5</v>
       </c>
-      <c r="J31" s="39" t="str">
+      <c r="J31" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26326,7 +26325,7 @@
         <f t="shared" si="2"/>
         <v>SW5</v>
       </c>
-      <c r="J32" s="39" t="str">
+      <c r="J32" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -26363,7 +26362,7 @@
         <f t="shared" si="2"/>
         <v>SW6</v>
       </c>
-      <c r="J33" s="39" t="str">
+      <c r="J33" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26400,7 +26399,7 @@
         <f t="shared" si="2"/>
         <v>SW6</v>
       </c>
-      <c r="J34" s="39" t="str">
+      <c r="J34" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26437,7 +26436,7 @@
         <f t="shared" si="2"/>
         <v>SW6</v>
       </c>
-      <c r="J35" s="39" t="str">
+      <c r="J35" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -26474,7 +26473,7 @@
         <f t="shared" si="2"/>
         <v>SW7</v>
       </c>
-      <c r="J36" s="39" t="str">
+      <c r="J36" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26511,7 +26510,7 @@
         <f t="shared" si="2"/>
         <v>SW7</v>
       </c>
-      <c r="J37" s="39" t="str">
+      <c r="J37" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26548,7 +26547,7 @@
         <f t="shared" si="2"/>
         <v>SW7</v>
       </c>
-      <c r="J38" s="39" t="str">
+      <c r="J38" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -26585,7 +26584,7 @@
         <f t="shared" si="2"/>
         <v>SW8</v>
       </c>
-      <c r="J39" s="39" t="str">
+      <c r="J39" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26622,7 +26621,7 @@
         <f t="shared" si="2"/>
         <v>SW8</v>
       </c>
-      <c r="J40" s="39" t="str">
+      <c r="J40" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26659,7 +26658,7 @@
         <f t="shared" si="2"/>
         <v>SW8</v>
       </c>
-      <c r="J41" s="39" t="str">
+      <c r="J41" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -26669,7 +26668,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B42" s="13" t="s">
@@ -26696,7 +26695,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J42" s="39" t="str">
+      <c r="J42" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26706,7 +26705,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="13" t="s">
@@ -26733,7 +26732,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J43" s="39" t="str">
+      <c r="J43" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26743,7 +26742,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="13" t="s">
@@ -26770,7 +26769,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J44" s="39" t="str">
+      <c r="J44" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -26780,7 +26779,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B45" s="13" t="s">
@@ -26807,7 +26806,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J45" s="39" t="str">
+      <c r="J45" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26817,7 +26816,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="13" t="s">
@@ -26844,7 +26843,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J46" s="39" t="str">
+      <c r="J46" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26854,7 +26853,7 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B47" s="13" t="s">
@@ -26881,7 +26880,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J47" s="39" t="str">
+      <c r="J47" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -26891,7 +26890,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="13" t="s">
@@ -26918,7 +26917,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J48" s="39" t="str">
+      <c r="J48" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -26928,7 +26927,7 @@
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="13" t="s">
@@ -26955,7 +26954,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J49" s="39" t="str">
+      <c r="J49" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -26965,7 +26964,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B50" s="13" t="s">
@@ -26992,7 +26991,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J50" s="39" t="str">
+      <c r="J50" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -27002,7 +27001,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B51" s="13" t="s">
@@ -27029,7 +27028,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J51" s="39" t="str">
+      <c r="J51" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -27039,7 +27038,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="32" t="s">
+      <c r="A52" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B52" s="13" t="s">
@@ -27066,7 +27065,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J52" s="39" t="str">
+      <c r="J52" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -27076,7 +27075,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B53" s="13" t="s">
@@ -27103,7 +27102,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J53" s="39" t="str">
+      <c r="J53" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -27113,7 +27112,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="32" t="s">
+      <c r="A54" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B54" s="13" t="s">
@@ -27140,7 +27139,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J54" s="39" t="str">
+      <c r="J54" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -27150,7 +27149,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="32" t="s">
+      <c r="A55" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B55" s="13" t="s">
@@ -27177,7 +27176,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J55" s="39" t="str">
+      <c r="J55" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -27187,7 +27186,7 @@
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B56" s="13" t="s">
@@ -27214,7 +27213,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J56" s="39" t="str">
+      <c r="J56" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -27224,7 +27223,7 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="32" t="s">
+      <c r="A57" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B57" s="13" t="s">
@@ -27251,7 +27250,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J57" s="39" t="str">
+      <c r="J57" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -27261,7 +27260,7 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="32" t="s">
+      <c r="A58" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="13" t="s">
@@ -27288,7 +27287,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J58" s="39" t="str">
+      <c r="J58" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -27298,7 +27297,7 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B59" s="13" t="s">
@@ -27325,7 +27324,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J59" s="39" t="str">
+      <c r="J59" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -27335,7 +27334,7 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="32" t="s">
+      <c r="A60" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B60" s="13" t="s">
@@ -27362,7 +27361,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J60" s="39" t="str">
+      <c r="J60" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -27372,7 +27371,7 @@
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="32" t="s">
+      <c r="A61" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B61" s="13" t="s">
@@ -27399,7 +27398,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J61" s="39" t="str">
+      <c r="J61" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -27409,7 +27408,7 @@
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="32" t="s">
+      <c r="A62" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B62" s="13" t="s">
@@ -27436,7 +27435,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J62" s="39" t="str">
+      <c r="J62" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -27446,7 +27445,7 @@
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B63" s="13" t="s">
@@ -27473,7 +27472,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J63" s="39" t="str">
+      <c r="J63" s="35" t="str">
         <f t="shared" si="3"/>
         <v>01</v>
       </c>
@@ -27483,7 +27482,7 @@
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="32" t="s">
+      <c r="A64" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B64" s="13" t="s">
@@ -27510,7 +27509,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J64" s="39" t="str">
+      <c r="J64" s="35" t="str">
         <f t="shared" si="3"/>
         <v>M</v>
       </c>
@@ -27520,7 +27519,7 @@
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="32" t="s">
+      <c r="A65" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B65" s="13" t="s">
@@ -27547,7 +27546,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J65" s="39" t="str">
+      <c r="J65" s="35" t="str">
         <f t="shared" si="3"/>
         <v>02</v>
       </c>
@@ -27557,7 +27556,7 @@
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="32" t="s">
+      <c r="A66" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B66" s="13" t="s">
@@ -27584,7 +27583,7 @@
         <f t="shared" si="2"/>
         <v>PGL</v>
       </c>
-      <c r="J66" s="39" t="str">
+      <c r="J66" s="35" t="str">
         <f t="shared" si="3"/>
         <v>03</v>
       </c>
@@ -27594,7 +27593,7 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B67" s="13" t="s">
@@ -27614,14 +27613,14 @@
         <v>135</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" ref="H67:H111" si="6">CONCATENATE(B67," Station - Level ",C67)</f>
+        <f t="shared" ref="H67:H84" si="6">CONCATENATE(B67," Station - Level ",C67)</f>
         <v>Teck Lee Station - Level 01</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I111" si="7">A67</f>
         <v>PGL</v>
       </c>
-      <c r="J67" s="39" t="str">
+      <c r="J67" s="35" t="str">
         <f t="shared" ref="J67:J111" si="8">C67</f>
         <v>01</v>
       </c>
@@ -27631,7 +27630,7 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="32" t="s">
+      <c r="A68" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B68" s="13" t="s">
@@ -27658,7 +27657,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J68" s="39" t="str">
+      <c r="J68" s="35" t="str">
         <f t="shared" si="8"/>
         <v>02</v>
       </c>
@@ -27668,7 +27667,7 @@
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B69" s="13" t="s">
@@ -27695,7 +27694,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J69" s="39" t="str">
+      <c r="J69" s="35" t="str">
         <f t="shared" si="8"/>
         <v>03</v>
       </c>
@@ -27705,7 +27704,7 @@
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A70" s="32" t="s">
+      <c r="A70" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B70" s="13" t="s">
@@ -27732,7 +27731,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J70" s="39" t="str">
+      <c r="J70" s="35" t="str">
         <f t="shared" si="8"/>
         <v>01</v>
       </c>
@@ -27742,7 +27741,7 @@
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="32" t="s">
+      <c r="A71" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B71" s="13" t="s">
@@ -27769,7 +27768,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J71" s="39" t="str">
+      <c r="J71" s="35" t="str">
         <f t="shared" si="8"/>
         <v>02</v>
       </c>
@@ -27779,7 +27778,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A72" s="32" t="s">
+      <c r="A72" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B72" s="13" t="s">
@@ -27806,7 +27805,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J72" s="39" t="str">
+      <c r="J72" s="35" t="str">
         <f t="shared" si="8"/>
         <v>03</v>
       </c>
@@ -27816,7 +27815,7 @@
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="32" t="s">
+      <c r="A73" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B73" s="13" t="s">
@@ -27843,7 +27842,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J73" s="39" t="str">
+      <c r="J73" s="35" t="str">
         <f t="shared" si="8"/>
         <v>01</v>
       </c>
@@ -27853,7 +27852,7 @@
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="32" t="s">
+      <c r="A74" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B74" s="13" t="s">
@@ -27880,7 +27879,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J74" s="39" t="str">
+      <c r="J74" s="35" t="str">
         <f t="shared" si="8"/>
         <v>02</v>
       </c>
@@ -27890,7 +27889,7 @@
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A75" s="32" t="s">
+      <c r="A75" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B75" s="13" t="s">
@@ -27917,7 +27916,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J75" s="39" t="str">
+      <c r="J75" s="35" t="str">
         <f t="shared" si="8"/>
         <v>03</v>
       </c>
@@ -27927,7 +27926,7 @@
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A76" s="32" t="s">
+      <c r="A76" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B76" s="13" t="s">
@@ -27954,7 +27953,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J76" s="39" t="str">
+      <c r="J76" s="35" t="str">
         <f t="shared" si="8"/>
         <v>01</v>
       </c>
@@ -27964,7 +27963,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A77" s="32" t="s">
+      <c r="A77" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B77" s="13" t="s">
@@ -27991,7 +27990,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J77" s="39" t="str">
+      <c r="J77" s="35" t="str">
         <f t="shared" si="8"/>
         <v>02</v>
       </c>
@@ -28001,7 +28000,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="32" t="s">
+      <c r="A78" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B78" s="13" t="s">
@@ -28028,7 +28027,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J78" s="39" t="str">
+      <c r="J78" s="35" t="str">
         <f t="shared" si="8"/>
         <v>03</v>
       </c>
@@ -28038,7 +28037,7 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A79" s="32" t="s">
+      <c r="A79" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B79" s="13" t="s">
@@ -28065,7 +28064,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J79" s="39" t="str">
+      <c r="J79" s="35" t="str">
         <f t="shared" si="8"/>
         <v>01</v>
       </c>
@@ -28075,7 +28074,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A80" s="32" t="s">
+      <c r="A80" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B80" s="13" t="s">
@@ -28102,7 +28101,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J80" s="39" t="str">
+      <c r="J80" s="35" t="str">
         <f t="shared" si="8"/>
         <v>02</v>
       </c>
@@ -28112,7 +28111,7 @@
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" s="32" t="s">
+      <c r="A81" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B81" s="13" t="s">
@@ -28139,7 +28138,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J81" s="39" t="str">
+      <c r="J81" s="35" t="str">
         <f t="shared" si="8"/>
         <v>03</v>
       </c>
@@ -28149,7 +28148,7 @@
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A82" s="32" t="s">
+      <c r="A82" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B82" s="13" t="s">
@@ -28176,7 +28175,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J82" s="39" t="str">
+      <c r="J82" s="35" t="str">
         <f t="shared" si="8"/>
         <v>01</v>
       </c>
@@ -28186,7 +28185,7 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" s="32" t="s">
+      <c r="A83" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B83" s="13" t="s">
@@ -28213,7 +28212,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J83" s="39" t="str">
+      <c r="J83" s="35" t="str">
         <f t="shared" si="8"/>
         <v>02</v>
       </c>
@@ -28223,7 +28222,7 @@
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A84" s="32" t="s">
+      <c r="A84" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B84" s="13" t="s">
@@ -28250,7 +28249,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J84" s="39" t="str">
+      <c r="J84" s="35" t="str">
         <f t="shared" si="8"/>
         <v>03</v>
       </c>
@@ -28260,7 +28259,7 @@
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85" s="32" t="s">
+      <c r="A85" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B85" s="13" t="s">
@@ -28287,7 +28286,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J85" s="39" t="str">
+      <c r="J85" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SE1</v>
       </c>
@@ -28297,7 +28296,7 @@
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86" s="32" t="s">
+      <c r="A86" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B86" s="13" t="s">
@@ -28324,7 +28323,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J86" s="39" t="str">
+      <c r="J86" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SE2</v>
       </c>
@@ -28334,7 +28333,7 @@
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A87" s="32" t="s">
+      <c r="A87" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B87" s="13" t="s">
@@ -28361,7 +28360,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J87" s="39" t="str">
+      <c r="J87" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SE3</v>
       </c>
@@ -28371,7 +28370,7 @@
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A88" s="32" t="s">
+      <c r="A88" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B88" s="13" t="s">
@@ -28398,7 +28397,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J88" s="39" t="str">
+      <c r="J88" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SE4</v>
       </c>
@@ -28408,7 +28407,7 @@
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A89" s="32" t="s">
+      <c r="A89" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B89" s="13" t="s">
@@ -28435,7 +28434,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J89" s="39" t="str">
+      <c r="J89" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SE5</v>
       </c>
@@ -28445,7 +28444,7 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A90" s="32" t="s">
+      <c r="A90" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B90" s="13" t="s">
@@ -28472,7 +28471,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J90" s="39" t="str">
+      <c r="J90" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SW1</v>
       </c>
@@ -28482,7 +28481,7 @@
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A91" s="32" t="s">
+      <c r="A91" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B91" s="13" t="s">
@@ -28509,7 +28508,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J91" s="39" t="str">
+      <c r="J91" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SW2</v>
       </c>
@@ -28519,7 +28518,7 @@
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A92" s="32" t="s">
+      <c r="A92" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B92" s="13" t="s">
@@ -28546,7 +28545,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J92" s="39" t="str">
+      <c r="J92" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SW3</v>
       </c>
@@ -28556,7 +28555,7 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="32" t="s">
+      <c r="A93" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B93" s="13" t="s">
@@ -28583,7 +28582,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J93" s="39" t="str">
+      <c r="J93" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SW4</v>
       </c>
@@ -28593,7 +28592,7 @@
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="32" t="s">
+      <c r="A94" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B94" s="13" t="s">
@@ -28620,7 +28619,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J94" s="39" t="str">
+      <c r="J94" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SW5</v>
       </c>
@@ -28630,7 +28629,7 @@
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="32" t="s">
+      <c r="A95" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B95" s="13" t="s">
@@ -28657,7 +28656,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J95" s="39" t="str">
+      <c r="J95" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SW6</v>
       </c>
@@ -28667,7 +28666,7 @@
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="32" t="s">
+      <c r="A96" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B96" s="13" t="s">
@@ -28694,7 +28693,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J96" s="39" t="str">
+      <c r="J96" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SW7</v>
       </c>
@@ -28704,7 +28703,7 @@
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A97" s="32" t="s">
+      <c r="A97" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B97" s="13" t="s">
@@ -28731,7 +28730,7 @@
         <f t="shared" si="7"/>
         <v>SKG</v>
       </c>
-      <c r="J97" s="39" t="str">
+      <c r="J97" s="35" t="str">
         <f t="shared" si="8"/>
         <v>SW8</v>
       </c>
@@ -28741,7 +28740,7 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="32" t="s">
+      <c r="A98" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B98" s="13" t="s">
@@ -28768,7 +28767,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J98" s="39" t="str">
+      <c r="J98" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PE1</v>
       </c>
@@ -28778,7 +28777,7 @@
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="32" t="s">
+      <c r="A99" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B99" s="13" t="s">
@@ -28805,7 +28804,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J99" s="39" t="str">
+      <c r="J99" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PE2</v>
       </c>
@@ -28815,7 +28814,7 @@
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100" s="32" t="s">
+      <c r="A100" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B100" s="13" t="s">
@@ -28842,7 +28841,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J100" s="39" t="str">
+      <c r="J100" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PE3</v>
       </c>
@@ -28852,7 +28851,7 @@
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A101" s="32" t="s">
+      <c r="A101" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B101" s="13" t="s">
@@ -28879,7 +28878,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J101" s="39" t="str">
+      <c r="J101" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PE4</v>
       </c>
@@ -28889,7 +28888,7 @@
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A102" s="32" t="s">
+      <c r="A102" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B102" s="13" t="s">
@@ -28916,7 +28915,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J102" s="39" t="str">
+      <c r="J102" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PE5</v>
       </c>
@@ -28926,7 +28925,7 @@
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103" s="32" t="s">
+      <c r="A103" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B103" s="13" t="s">
@@ -28953,7 +28952,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J103" s="39" t="str">
+      <c r="J103" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PE6</v>
       </c>
@@ -28963,7 +28962,7 @@
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="32" t="s">
+      <c r="A104" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B104" s="13" t="s">
@@ -28990,7 +28989,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J104" s="39" t="str">
+      <c r="J104" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PE7</v>
       </c>
@@ -29000,7 +28999,7 @@
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A105" s="32" t="s">
+      <c r="A105" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B105" s="13" t="s">
@@ -29027,7 +29026,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J105" s="39" t="str">
+      <c r="J105" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PW1</v>
       </c>
@@ -29037,7 +29036,7 @@
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A106" s="32" t="s">
+      <c r="A106" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B106" s="13" t="s">
@@ -29064,7 +29063,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J106" s="39" t="str">
+      <c r="J106" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PW2</v>
       </c>
@@ -29074,7 +29073,7 @@
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A107" s="32" t="s">
+      <c r="A107" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B107" s="13" t="s">
@@ -29101,7 +29100,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J107" s="39" t="str">
+      <c r="J107" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PW3</v>
       </c>
@@ -29111,7 +29110,7 @@
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A108" s="32" t="s">
+      <c r="A108" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B108" s="13" t="s">
@@ -29138,7 +29137,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J108" s="39" t="str">
+      <c r="J108" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PW4</v>
       </c>
@@ -29148,7 +29147,7 @@
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A109" s="32" t="s">
+      <c r="A109" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B109" s="13" t="s">
@@ -29175,7 +29174,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J109" s="39" t="str">
+      <c r="J109" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PW5</v>
       </c>
@@ -29185,7 +29184,7 @@
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A110" s="32" t="s">
+      <c r="A110" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B110" s="13" t="s">
@@ -29212,7 +29211,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J110" s="39" t="str">
+      <c r="J110" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PW6</v>
       </c>
@@ -29222,7 +29221,7 @@
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A111" s="32" t="s">
+      <c r="A111" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B111" s="13" t="s">
@@ -29249,7 +29248,7 @@
         <f t="shared" si="7"/>
         <v>PGL</v>
       </c>
-      <c r="J111" s="39" t="str">
+      <c r="J111" s="35" t="str">
         <f t="shared" si="8"/>
         <v>PW7</v>
       </c>
@@ -44938,7 +44937,7 @@
       <c r="I2721" t="s">
         <v>43</v>
       </c>
-      <c r="J2721" s="39" t="s">
+      <c r="J2721" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2721" t="s">
@@ -44971,7 +44970,7 @@
       <c r="I2722" t="s">
         <v>45</v>
       </c>
-      <c r="J2722" s="39" t="s">
+      <c r="J2722" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2722" t="s">
@@ -45004,7 +45003,7 @@
       <c r="I2723" t="s">
         <v>47</v>
       </c>
-      <c r="J2723" s="39" t="s">
+      <c r="J2723" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2723" t="s">
@@ -45037,7 +45036,7 @@
       <c r="I2724" t="s">
         <v>49</v>
       </c>
-      <c r="J2724" s="39" t="s">
+      <c r="J2724" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2724" t="s">
@@ -45070,7 +45069,7 @@
       <c r="I2725" t="s">
         <v>51</v>
       </c>
-      <c r="J2725" s="39" t="s">
+      <c r="J2725" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2725" t="s">
@@ -45103,7 +45102,7 @@
       <c r="I2726" t="s">
         <v>53</v>
       </c>
-      <c r="J2726" s="39" t="s">
+      <c r="J2726" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2726" t="s">
@@ -45136,7 +45135,7 @@
       <c r="I2727" t="s">
         <v>55</v>
       </c>
-      <c r="J2727" s="39" t="s">
+      <c r="J2727" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2727" t="s">
@@ -45169,7 +45168,7 @@
       <c r="I2728" t="s">
         <v>57</v>
       </c>
-      <c r="J2728" s="39" t="s">
+      <c r="J2728" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2728" t="s">
@@ -45202,7 +45201,7 @@
       <c r="I2729" t="s">
         <v>59</v>
       </c>
-      <c r="J2729" s="39" t="s">
+      <c r="J2729" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2729" t="s">
@@ -45235,7 +45234,7 @@
       <c r="I2730" t="s">
         <v>61</v>
       </c>
-      <c r="J2730" s="39" t="s">
+      <c r="J2730" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2730" t="s">
@@ -45268,7 +45267,7 @@
       <c r="I2731" t="s">
         <v>63</v>
       </c>
-      <c r="J2731" s="39" t="s">
+      <c r="J2731" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2731" t="s">
@@ -45301,7 +45300,7 @@
       <c r="I2732" t="s">
         <v>65</v>
       </c>
-      <c r="J2732" s="39" t="s">
+      <c r="J2732" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2732" t="s">
@@ -45334,7 +45333,7 @@
       <c r="I2733" t="s">
         <v>67</v>
       </c>
-      <c r="J2733" s="39" t="s">
+      <c r="J2733" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2733" t="s">
@@ -45367,7 +45366,7 @@
       <c r="I2734" t="s">
         <v>11</v>
       </c>
-      <c r="J2734" s="39" t="s">
+      <c r="J2734" s="35" t="s">
         <v>864</v>
       </c>
       <c r="L2734" t="s">
@@ -45376,8 +45375,8 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45850,7 +45849,7 @@
       <c r="A1" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>138</v>
       </c>
     </row>
@@ -45858,7 +45857,7 @@
       <c r="A2" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="37"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
@@ -49326,7 +49325,7 @@
       <c r="A1" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>560</v>
       </c>
     </row>
@@ -49334,7 +49333,7 @@
       <c r="A2" s="23" t="s">
         <v>559</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="39"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">

</xml_diff>